<commit_message>
upd to crossing data and results
</commit_message>
<xml_diff>
--- a/data/Experiment_table_Ecy_2023.xlsx
+++ b/data/Experiment_table_Ecy_2023.xlsx
@@ -11,22 +11,22 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$XFD$233</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$XFD$278</definedName>
   </definedNames>
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1713512347" val="1050" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1713512347" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1713512347" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1713512347"/>
+      <pm:revision xmlns:pm="smNativeData" day="1717669421" val="1050" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1717669421" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1717669421" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1717669421"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -159,6 +159,30 @@
   <si>
     <t>one of the dead is female with eggs</t>
   </si>
+  <si>
+    <t>females in amplexus with black (maybe marble) eggs</t>
+  </si>
+  <si>
+    <t>female in amplexus with black (maybe marble) eggs</t>
+  </si>
+  <si>
+    <t>female in amplexus with "comma" eggs</t>
+  </si>
+  <si>
+    <t>one free female with marble eggs; one female in amplesus with marble eggs</t>
+  </si>
+  <si>
+    <t>female in amplexus with marble eggs</t>
+  </si>
+  <si>
+    <t>free ovigerous females: 2 orange + 1 marble</t>
+  </si>
+  <si>
+    <t>free ovigerous females: 1 orange + 2 marble</t>
+  </si>
+  <si>
+    <t>free females: 2 w/black eggs; one marble; one with juveniles</t>
+  </si>
 </sst>
 </file>
 
@@ -183,7 +207,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1713512347" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1717669421" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -198,7 +222,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1713512347" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1717669421" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -213,7 +237,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1713512347" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1717669421" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -244,7 +268,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1713512347" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1717669421" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -266,7 +290,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1713512347"/>
+          <pm:border xmlns:pm="smNativeData" id="1717669421"/>
         </ext>
       </extLst>
     </border>
@@ -285,7 +309,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1713512347">
+          <pm:border xmlns:pm="smNativeData" id="1717669421">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -306,7 +330,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1713512347">
+          <pm:border xmlns:pm="smNativeData" id="1717669421">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -327,7 +351,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1713512347">
+          <pm:border xmlns:pm="smNativeData" id="1717669421">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -348,7 +372,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1713512347"/>
+          <pm:border xmlns:pm="smNativeData" id="1717669421"/>
         </ext>
       </extLst>
     </border>
@@ -356,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -383,12 +407,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -396,7 +428,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1713512347" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1717669421" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -661,11 +693,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L318"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" zoomScale="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B226" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="K259" sqref="K259"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B286" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H291" sqref="H291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -5616,7 +5648,7 @@
       </c>
     </row>
     <row r="158" spans="1:11" s="3" customFormat="1" ht="13.60">
-      <c r="A158" s="18" t="n">
+      <c r="A158" s="4" t="n">
         <v>45258</v>
       </c>
       <c r="C158" s="3" t="s">
@@ -5631,7 +5663,6 @@
       <c r="F158" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G158" s="19"/>
       <c r="H158" s="3" t="n">
         <v>0</v>
       </c>
@@ -7753,32 +7784,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:11" s="15" customFormat="1" ht="13.60">
-      <c r="A238" s="16" t="n">
+    <row r="238" spans="1:11" s="3" customFormat="1" ht="13.60">
+      <c r="A238" s="4" t="n">
         <v>45370</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D238" s="17" t="n">
+      <c r="D238" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="E238" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F238" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H238" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I238" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J238" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K238" s="15" t="n">
+      <c r="E238" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F238" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H238" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I238" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J238" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K238" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7898,32 +7929,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:11" s="15" customFormat="1" ht="13.60">
-      <c r="A243" s="16" t="n">
+    <row r="243" spans="1:11" s="3" customFormat="1" ht="13.60">
+      <c r="A243" s="4" t="n">
         <v>45377</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D243" s="17" t="n">
+      <c r="D243" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="E243" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F243" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H243" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I243" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="J243" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K243" s="15" t="n">
+      <c r="E243" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F243" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H243" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I243" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J243" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K243" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8043,32 +8074,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:11" s="15" customFormat="1" ht="13.60">
-      <c r="A248" s="16" t="n">
+    <row r="248" spans="1:11" s="3" customFormat="1" ht="13.60">
+      <c r="A248" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D248" s="17" t="n">
+      <c r="D248" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="E248" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F248" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H248" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I248" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="J248" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K248" s="15" t="n">
+      <c r="E248" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F248" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H248" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I248" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J248" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K248" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8185,32 +8216,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:11" s="15" customFormat="1" ht="13.60">
-      <c r="A253" s="16" t="n">
+    <row r="253" spans="1:11" s="3" customFormat="1" ht="13.60">
+      <c r="A253" s="4" t="n">
         <v>45391</v>
       </c>
       <c r="C253" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D253" s="17" t="n">
+      <c r="D253" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="E253" s="15" t="n">
+      <c r="E253" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F253" s="15" t="n">
+      <c r="F253" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H253" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I253" s="15" t="n">
+      <c r="H253" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I253" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="J253" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K253" s="15" t="n">
+      <c r="J253" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K253" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8330,174 +8361,994 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:11" s="15" customFormat="1" ht="13.60">
-      <c r="A258" s="16" t="n">
+    <row r="258" spans="1:11" s="3" customFormat="1" ht="13.60">
+      <c r="A258" s="4" t="n">
         <v>45398</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D258" s="17" t="n">
+      <c r="D258" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="E258" s="15" t="n">
+      <c r="E258" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F258" s="15" t="n">
+      <c r="F258" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H258" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I258" s="15" t="n">
+      <c r="H258" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I258" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="J258" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="K258" s="15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="1:4">
-      <c r="A259" s="1"/>
-      <c r="D259" s="5"/>
-    </row>
-    <row r="260" spans="1:4">
-      <c r="A260" s="2"/>
-      <c r="D260" s="5"/>
-    </row>
-    <row r="261" spans="1:4">
-      <c r="A261" s="2"/>
-      <c r="D261" s="5"/>
-    </row>
-    <row r="262" spans="1:4" s="0" customFormat="1">
-      <c r="A262" s="2"/>
-      <c r="D262" s="5"/>
-    </row>
-    <row r="263" spans="1:4">
-      <c r="A263" s="2"/>
-      <c r="D263" s="5"/>
-    </row>
-    <row r="264" spans="1:4">
-      <c r="A264" s="2"/>
-      <c r="D264" s="5"/>
-    </row>
-    <row r="265" spans="1:4">
-      <c r="A265" s="2"/>
-      <c r="D265" s="5"/>
-    </row>
-    <row r="266" spans="1:4" s="0" customFormat="1">
-      <c r="A266" s="2"/>
-      <c r="D266" s="5"/>
-    </row>
-    <row r="267" spans="1:4">
-      <c r="A267" s="1"/>
-      <c r="D267" s="5"/>
-    </row>
-    <row r="268" spans="1:4">
-      <c r="A268" s="1"/>
-      <c r="D268" s="5"/>
-    </row>
-    <row r="269" spans="1:4">
-      <c r="A269" s="1"/>
-      <c r="D269" s="5"/>
-    </row>
-    <row r="270" spans="1:4" s="0" customFormat="1">
-      <c r="A270" s="1"/>
-      <c r="D270" s="5"/>
-    </row>
-    <row r="271" spans="1:4" s="0" customFormat="1">
-      <c r="A271" s="1"/>
-      <c r="D271" s="5"/>
-    </row>
-    <row r="272" spans="1:4">
-      <c r="A272" s="1"/>
-      <c r="D272" s="5"/>
-    </row>
-    <row r="273" spans="1:4">
-      <c r="A273" s="1"/>
-      <c r="D273" s="5"/>
-    </row>
-    <row r="274" spans="1:4" s="0" customFormat="1">
-      <c r="A274" s="1"/>
-      <c r="D274" s="5"/>
-    </row>
-    <row r="275" spans="1:4" s="0" customFormat="1">
-      <c r="A275" s="1"/>
-      <c r="D275" s="5"/>
-    </row>
-    <row r="276" spans="1:4" s="0" customFormat="1">
-      <c r="A276" s="1"/>
-      <c r="D276" s="5"/>
-    </row>
-    <row r="277" spans="1:4" s="0" customFormat="1">
-      <c r="A277" s="1"/>
-      <c r="D277" s="5"/>
-    </row>
-    <row r="278" spans="1:4" s="0" customFormat="1">
-      <c r="A278" s="1"/>
-      <c r="D278" s="5"/>
-    </row>
-    <row r="279" spans="1:4">
-      <c r="A279" s="1"/>
-      <c r="D279" s="5"/>
-    </row>
-    <row r="280" spans="1:4">
-      <c r="A280" s="1"/>
-      <c r="D280" s="5"/>
-    </row>
-    <row r="281" spans="1:4">
-      <c r="A281" s="1"/>
-      <c r="D281" s="5"/>
-    </row>
-    <row r="282" spans="1:4" s="0" customFormat="1">
-      <c r="A282" s="1"/>
-      <c r="D282" s="5"/>
-    </row>
-    <row r="283" spans="1:4">
-      <c r="A283" s="1"/>
-      <c r="D283" s="5"/>
-    </row>
-    <row r="284" spans="1:4">
-      <c r="A284" s="1"/>
-      <c r="D284" s="5"/>
-    </row>
-    <row r="285" spans="1:4">
-      <c r="A285" s="1"/>
-      <c r="D285" s="5"/>
-    </row>
-    <row r="286" spans="1:4" s="0" customFormat="1">
-      <c r="A286" s="1"/>
-      <c r="D286" s="5"/>
-    </row>
-    <row r="287" spans="1:4">
-      <c r="A287" s="1"/>
-      <c r="D287" s="5"/>
-    </row>
-    <row r="288" spans="1:4">
-      <c r="A288" s="1"/>
-      <c r="D288" s="5"/>
-    </row>
-    <row r="289" spans="1:4">
-      <c r="A289" s="1"/>
-      <c r="D289" s="5"/>
-    </row>
-    <row r="290" spans="1:4" s="0" customFormat="1">
-      <c r="A290" s="1"/>
-      <c r="D290" s="5"/>
-    </row>
-    <row r="291" spans="1:4">
-      <c r="A291" s="1"/>
-      <c r="D291" s="5"/>
-    </row>
-    <row r="292" spans="1:4">
-      <c r="A292" s="1"/>
-      <c r="D292" s="5"/>
-    </row>
-    <row r="293" spans="1:4">
-      <c r="A293" s="1"/>
-      <c r="D293" s="5"/>
+      <c r="J258" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K258" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11">
+      <c r="A259" s="1" t="n">
+        <v>45405</v>
+      </c>
+      <c r="C259" t="s">
+        <v>13</v>
+      </c>
+      <c r="D259" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="E259" t="n">
+        <v>1</v>
+      </c>
+      <c r="F259">
+        <f>SUM(G259:I259)</f>
+        <v>2</v>
+      </c>
+      <c r="I259" t="n">
+        <v>2</v>
+      </c>
+      <c r="J259" t="n">
+        <v>0</v>
+      </c>
+      <c r="K259" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11">
+      <c r="A260" s="1" t="n">
+        <v>45405</v>
+      </c>
+      <c r="C260" t="s">
+        <v>14</v>
+      </c>
+      <c r="D260" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E260" t="n">
+        <v>0</v>
+      </c>
+      <c r="F260">
+        <f>SUM(G260:I260)</f>
+        <v>2</v>
+      </c>
+      <c r="I260" t="n">
+        <v>2</v>
+      </c>
+      <c r="J260" t="n">
+        <v>0</v>
+      </c>
+      <c r="K260" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11">
+      <c r="A261" s="1" t="n">
+        <v>45405</v>
+      </c>
+      <c r="C261" t="s">
+        <v>15</v>
+      </c>
+      <c r="D261" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E261" t="n">
+        <v>1</v>
+      </c>
+      <c r="F261">
+        <f>SUM(G261:I261)</f>
+        <v>5</v>
+      </c>
+      <c r="I261" t="n">
+        <v>5</v>
+      </c>
+      <c r="J261" t="n">
+        <v>0</v>
+      </c>
+      <c r="K261" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" s="0" customFormat="1">
+      <c r="A262" s="1" t="n">
+        <v>45405</v>
+      </c>
+      <c r="C262" t="s">
+        <v>16</v>
+      </c>
+      <c r="D262" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E262" t="n">
+        <v>0</v>
+      </c>
+      <c r="F262">
+        <f>SUM(G262:I262)</f>
+        <v>0</v>
+      </c>
+      <c r="I262" t="n">
+        <v>0</v>
+      </c>
+      <c r="J262" t="n">
+        <v>0</v>
+      </c>
+      <c r="K262" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11">
+      <c r="A263" s="1" t="n">
+        <v>45405</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D263" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E263" t="n">
+        <v>3</v>
+      </c>
+      <c r="F263">
+        <f>SUM(G263:I263)</f>
+        <v>2</v>
+      </c>
+      <c r="I263" t="n">
+        <v>2</v>
+      </c>
+      <c r="J263" t="n">
+        <v>0</v>
+      </c>
+      <c r="K263" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11">
+      <c r="A264" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="C264" t="s">
+        <v>13</v>
+      </c>
+      <c r="D264" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="E264" t="n">
+        <v>2</v>
+      </c>
+      <c r="F264">
+        <f>SUM(G264:I264)</f>
+        <v>1</v>
+      </c>
+      <c r="I264" t="n">
+        <v>1</v>
+      </c>
+      <c r="J264" t="n">
+        <v>0</v>
+      </c>
+      <c r="K264" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11">
+      <c r="A265" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="C265" t="s">
+        <v>14</v>
+      </c>
+      <c r="D265" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E265" t="n">
+        <v>0</v>
+      </c>
+      <c r="F265">
+        <f>SUM(G265:I265)</f>
+        <v>2</v>
+      </c>
+      <c r="I265" t="n">
+        <v>2</v>
+      </c>
+      <c r="J265" t="n">
+        <v>0</v>
+      </c>
+      <c r="K265" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" s="0" customFormat="1">
+      <c r="A266" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="C266" t="s">
+        <v>15</v>
+      </c>
+      <c r="D266" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E266" t="n">
+        <v>1</v>
+      </c>
+      <c r="F266">
+        <f>SUM(G266:I266)</f>
+        <v>5</v>
+      </c>
+      <c r="I266" t="n">
+        <v>5</v>
+      </c>
+      <c r="J266" t="n">
+        <v>0</v>
+      </c>
+      <c r="K266" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11">
+      <c r="A267" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="C267" t="s">
+        <v>16</v>
+      </c>
+      <c r="D267" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E267" t="n">
+        <v>0</v>
+      </c>
+      <c r="F267">
+        <f>SUM(G267:I267)</f>
+        <v>0</v>
+      </c>
+      <c r="I267" t="n">
+        <v>0</v>
+      </c>
+      <c r="J267" t="n">
+        <v>0</v>
+      </c>
+      <c r="K267" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11">
+      <c r="A268" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="C268" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D268" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E268" t="n">
+        <v>2</v>
+      </c>
+      <c r="F268">
+        <f>SUM(G268:I268)</f>
+        <v>3</v>
+      </c>
+      <c r="I268" t="n">
+        <v>3</v>
+      </c>
+      <c r="J268" t="n">
+        <v>0</v>
+      </c>
+      <c r="K268" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11">
+      <c r="A269" s="1" t="n">
+        <v>45419</v>
+      </c>
+      <c r="C269" t="s">
+        <v>13</v>
+      </c>
+      <c r="D269" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="E269" t="n">
+        <v>2</v>
+      </c>
+      <c r="F269">
+        <f>SUM(G269:I269)</f>
+        <v>1</v>
+      </c>
+      <c r="I269" t="n">
+        <v>1</v>
+      </c>
+      <c r="J269" t="n">
+        <v>0</v>
+      </c>
+      <c r="K269" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" s="0" customFormat="1">
+      <c r="A270" s="1" t="n">
+        <v>45419</v>
+      </c>
+      <c r="C270" t="s">
+        <v>14</v>
+      </c>
+      <c r="D270" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E270" t="n">
+        <v>1</v>
+      </c>
+      <c r="F270">
+        <f>SUM(G270:I270)</f>
+        <v>1</v>
+      </c>
+      <c r="I270" t="n">
+        <v>1</v>
+      </c>
+      <c r="J270" t="n">
+        <v>1</v>
+      </c>
+      <c r="K270" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" s="0" customFormat="1">
+      <c r="A271" s="1" t="n">
+        <v>45419</v>
+      </c>
+      <c r="C271" t="s">
+        <v>15</v>
+      </c>
+      <c r="D271" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E271" t="n">
+        <v>3</v>
+      </c>
+      <c r="F271">
+        <f>SUM(G271:I271)</f>
+        <v>5</v>
+      </c>
+      <c r="G271" t="n">
+        <v>2</v>
+      </c>
+      <c r="I271" t="n">
+        <v>3</v>
+      </c>
+      <c r="J271" t="n">
+        <v>0</v>
+      </c>
+      <c r="K271" t="n">
+        <v>0</v>
+      </c>
+      <c r="L271" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11">
+      <c r="A272" s="1" t="n">
+        <v>45419</v>
+      </c>
+      <c r="C272" t="s">
+        <v>16</v>
+      </c>
+      <c r="D272" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E272" t="n">
+        <v>0</v>
+      </c>
+      <c r="F272">
+        <f>SUM(G272:I272)</f>
+        <v>0</v>
+      </c>
+      <c r="I272" t="n">
+        <v>0</v>
+      </c>
+      <c r="J272" t="n">
+        <v>0</v>
+      </c>
+      <c r="K272" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12">
+      <c r="A273" s="1" t="n">
+        <v>45419</v>
+      </c>
+      <c r="C273" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D273" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E273" t="n">
+        <v>3</v>
+      </c>
+      <c r="F273">
+        <f>SUM(G273:I273)</f>
+        <v>4</v>
+      </c>
+      <c r="G273" t="n">
+        <v>1</v>
+      </c>
+      <c r="I273" t="n">
+        <v>3</v>
+      </c>
+      <c r="J273" t="n">
+        <v>0</v>
+      </c>
+      <c r="K273" t="n">
+        <v>0</v>
+      </c>
+      <c r="L273" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" s="0" customFormat="1">
+      <c r="A274" s="1" t="n">
+        <v>45426</v>
+      </c>
+      <c r="C274" t="s">
+        <v>13</v>
+      </c>
+      <c r="D274" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="E274" t="n">
+        <v>3</v>
+      </c>
+      <c r="F274">
+        <f>SUM(G274:I274)</f>
+        <v>1</v>
+      </c>
+      <c r="G274" t="n">
+        <v>1</v>
+      </c>
+      <c r="I274" t="n">
+        <v>0</v>
+      </c>
+      <c r="J274" t="n">
+        <v>0</v>
+      </c>
+      <c r="K274" t="n">
+        <v>0</v>
+      </c>
+      <c r="L274" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" s="0" customFormat="1">
+      <c r="A275" s="1" t="n">
+        <v>45426</v>
+      </c>
+      <c r="C275" t="s">
+        <v>14</v>
+      </c>
+      <c r="D275" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E275" t="n">
+        <v>3</v>
+      </c>
+      <c r="F275">
+        <f>SUM(G275:I275)</f>
+        <v>1</v>
+      </c>
+      <c r="I275" t="n">
+        <v>1</v>
+      </c>
+      <c r="J275" t="n">
+        <v>0</v>
+      </c>
+      <c r="K275" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" s="0" customFormat="1">
+      <c r="A276" s="1" t="n">
+        <v>45426</v>
+      </c>
+      <c r="C276" t="s">
+        <v>15</v>
+      </c>
+      <c r="D276" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E276" t="n">
+        <v>2</v>
+      </c>
+      <c r="F276">
+        <f>SUM(G276:I276)</f>
+        <v>5</v>
+      </c>
+      <c r="G276" t="n">
+        <v>1</v>
+      </c>
+      <c r="I276" t="n">
+        <v>4</v>
+      </c>
+      <c r="J276" t="n">
+        <v>0</v>
+      </c>
+      <c r="K276" t="n">
+        <v>3</v>
+      </c>
+      <c r="L276" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" s="0" customFormat="1">
+      <c r="A277" s="1" t="n">
+        <v>45426</v>
+      </c>
+      <c r="C277" t="s">
+        <v>16</v>
+      </c>
+      <c r="D277" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E277" t="n">
+        <v>0</v>
+      </c>
+      <c r="F277">
+        <f>SUM(G277:I277)</f>
+        <v>0</v>
+      </c>
+      <c r="I277" t="n">
+        <v>0</v>
+      </c>
+      <c r="J277" t="n">
+        <v>0</v>
+      </c>
+      <c r="K277" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" s="15" customFormat="1" ht="13.60">
+      <c r="A278" s="16" t="n">
+        <v>45426</v>
+      </c>
+      <c r="C278" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D278" s="17" t="n">
+        <v>20</v>
+      </c>
+      <c r="E278" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F278" s="22">
+        <f>SUM(G278:I278)</f>
+        <v>1</v>
+      </c>
+      <c r="I278" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J278" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K278" s="15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11">
+      <c r="A279" s="1" t="n">
+        <v>45433</v>
+      </c>
+      <c r="C279" t="s">
+        <v>13</v>
+      </c>
+      <c r="D279" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="E279" t="n">
+        <v>2</v>
+      </c>
+      <c r="F279" s="22">
+        <f>SUM(G279:I279)</f>
+        <v>2</v>
+      </c>
+      <c r="G279" t="n">
+        <v>1</v>
+      </c>
+      <c r="H279" t="n">
+        <v>0</v>
+      </c>
+      <c r="I279" t="n">
+        <v>1</v>
+      </c>
+      <c r="K279" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11">
+      <c r="A280" s="1" t="n">
+        <v>45433</v>
+      </c>
+      <c r="C280" t="s">
+        <v>14</v>
+      </c>
+      <c r="D280" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E280" t="n">
+        <v>3</v>
+      </c>
+      <c r="F280" s="22">
+        <f>SUM(G280:I280)</f>
+        <v>1</v>
+      </c>
+      <c r="I280" t="n">
+        <v>1</v>
+      </c>
+      <c r="K280" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11">
+      <c r="A281" s="1" t="n">
+        <v>45433</v>
+      </c>
+      <c r="C281" t="s">
+        <v>15</v>
+      </c>
+      <c r="D281" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E281" t="n">
+        <v>4</v>
+      </c>
+      <c r="F281" s="22">
+        <f>SUM(G281:I281)</f>
+        <v>2</v>
+      </c>
+      <c r="I281" t="n">
+        <v>2</v>
+      </c>
+      <c r="K281" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" s="0" customFormat="1">
+      <c r="A282" s="1" t="n">
+        <v>45433</v>
+      </c>
+      <c r="C282" t="s">
+        <v>16</v>
+      </c>
+      <c r="D282" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E282" t="n">
+        <v>0</v>
+      </c>
+      <c r="F282" s="22">
+        <f>SUM(G282:I282)</f>
+        <v>0</v>
+      </c>
+      <c r="I282" t="n">
+        <v>0</v>
+      </c>
+      <c r="K282" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" s="18" customFormat="1" ht="13.60">
+      <c r="A283" s="19" t="n">
+        <v>45433</v>
+      </c>
+      <c r="C283" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D283" s="17" t="n">
+        <v>19</v>
+      </c>
+      <c r="E283" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F283" s="22">
+        <f>SUM(G283:I283)</f>
+        <v>4</v>
+      </c>
+      <c r="G283" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H283" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I283" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K283" s="15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11">
+      <c r="A284" s="1" t="n">
+        <v>45440</v>
+      </c>
+      <c r="C284" t="s">
+        <v>13</v>
+      </c>
+      <c r="D284" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="E284" t="n">
+        <v>2</v>
+      </c>
+      <c r="F284" s="22">
+        <f>SUM(G284:I284)</f>
+        <v>1</v>
+      </c>
+      <c r="I284" t="n">
+        <v>1</v>
+      </c>
+      <c r="K284" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12">
+      <c r="A285" s="1" t="n">
+        <v>45440</v>
+      </c>
+      <c r="C285" t="s">
+        <v>14</v>
+      </c>
+      <c r="D285" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E285" t="n">
+        <v>4</v>
+      </c>
+      <c r="F285" s="22">
+        <f>SUM(G285:I285)</f>
+        <v>1</v>
+      </c>
+      <c r="G285" t="n">
+        <v>1</v>
+      </c>
+      <c r="I285" t="n">
+        <v>0</v>
+      </c>
+      <c r="K285" t="n">
+        <v>0</v>
+      </c>
+      <c r="L285" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" s="0" customFormat="1">
+      <c r="A286" s="1" t="n">
+        <v>45440</v>
+      </c>
+      <c r="C286" t="s">
+        <v>15</v>
+      </c>
+      <c r="D286" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E286" t="n">
+        <v>3</v>
+      </c>
+      <c r="F286" s="22">
+        <f>SUM(G286:I286)</f>
+        <v>6</v>
+      </c>
+      <c r="G286" t="n">
+        <v>3</v>
+      </c>
+      <c r="H286" t="n">
+        <v>3</v>
+      </c>
+      <c r="I286" t="n">
+        <v>0</v>
+      </c>
+      <c r="K286" t="n">
+        <v>0</v>
+      </c>
+      <c r="L286" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11">
+      <c r="A287" s="1" t="n">
+        <v>45440</v>
+      </c>
+      <c r="C287" t="s">
+        <v>16</v>
+      </c>
+      <c r="D287" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E287" t="n">
+        <v>0</v>
+      </c>
+      <c r="F287" s="22">
+        <f>SUM(G287:I287)</f>
+        <v>0</v>
+      </c>
+      <c r="K287" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" s="20" customFormat="1" ht="13.60">
+      <c r="A288" s="21" t="n">
+        <v>45440</v>
+      </c>
+      <c r="C288" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D288" s="17" t="n">
+        <v>19</v>
+      </c>
+      <c r="E288" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F288" s="22">
+        <f>SUM(G288:I288)</f>
+        <v>4</v>
+      </c>
+      <c r="G288" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H288" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="K288" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L288" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11">
+      <c r="A289" s="1" t="n">
+        <v>45447</v>
+      </c>
+      <c r="C289" t="s">
+        <v>13</v>
+      </c>
+      <c r="D289" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="E289" t="n">
+        <v>2</v>
+      </c>
+      <c r="F289" s="22">
+        <f>SUM(G289:I289)</f>
+        <v>3</v>
+      </c>
+      <c r="G289" t="n">
+        <v>2</v>
+      </c>
+      <c r="I289" t="n">
+        <v>1</v>
+      </c>
+      <c r="K289" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" s="0" customFormat="1">
+      <c r="A290" s="1" t="n">
+        <v>45447</v>
+      </c>
+      <c r="C290" t="s">
+        <v>14</v>
+      </c>
+      <c r="D290" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E290" t="n">
+        <v>4</v>
+      </c>
+      <c r="F290" s="22">
+        <f>SUM(G290:I290)</f>
+        <v>0</v>
+      </c>
+      <c r="K290" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11">
+      <c r="A291" s="1" t="n">
+        <v>45447</v>
+      </c>
+      <c r="C291" t="s">
+        <v>15</v>
+      </c>
+      <c r="D291" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E291" t="n">
+        <v>5</v>
+      </c>
+      <c r="F291" s="22">
+        <f>SUM(G291:I291)</f>
+        <v>6</v>
+      </c>
+      <c r="G291" t="n">
+        <v>5</v>
+      </c>
+      <c r="I291" t="n">
+        <v>1</v>
+      </c>
+      <c r="K291" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11">
+      <c r="A292" s="1" t="n">
+        <v>45447</v>
+      </c>
+      <c r="C292" t="s">
+        <v>16</v>
+      </c>
+      <c r="D292" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E292" t="n">
+        <v>0</v>
+      </c>
+      <c r="F292" s="22">
+        <f>SUM(G292:I292)</f>
+        <v>0</v>
+      </c>
+      <c r="K292" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" s="23" customFormat="1" ht="13.60">
+      <c r="A293" s="24" t="n">
+        <v>45447</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D293" s="25" t="n">
+        <v>18</v>
+      </c>
+      <c r="E293" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F293" s="15">
+        <f>SUM(G293:I293)</f>
+        <v>4</v>
+      </c>
+      <c r="H293" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I293" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K293" s="23" t="n">
+        <v>6</v>
+      </c>
+      <c r="L293" s="15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="294" spans="1:12" s="0" customFormat="1">
       <c r="A294" s="1"/>
@@ -8656,11 +9507,11 @@
       <c r="L318" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:XFD233"/>
+  <autoFilter ref="A1:XFD278"/>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1713512347" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1717669421" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -8669,14 +9520,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1713512347" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1713512347" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1717669421" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1717669421" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1713512347" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1717669421" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>